<commit_message>
fix typos, added more configs.
</commit_message>
<xml_diff>
--- a/modelCatalog/instances/Variables/PIHM_output.xlsx
+++ b/modelCatalog/instances/Variables/PIHM_output.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -591,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
more dataset spec and variables
</commit_message>
<xml_diff>
--- a/modelCatalog/instances/Variables/PIHM_output.xlsx
+++ b/modelCatalog/instances/Variables/PIHM_output.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10740" yWindow="1704" windowWidth="23220" windowHeight="15636"/>
+    <workbookView minimized="1" xWindow="10740" yWindow="1704" windowWidth="23220" windowHeight="15636"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="61">
   <si>
     <t>Interception storage</t>
   </si>
@@ -208,14 +208,17 @@
     <t>.rivFlx10</t>
   </si>
   <si>
-    <t>land_surface_water, depth</t>
+    <t>land_surface_water__depth</t>
+  </si>
+  <si>
+    <t>groundwater__head</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -248,6 +251,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -269,12 +277,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,16 +602,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
     <col min="3" max="3" width="38.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -629,7 +640,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -645,7 +656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -661,7 +672,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -679,7 +690,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -695,7 +706,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -705,13 +716,15 @@
       <c r="D6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -727,7 +740,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -743,7 +756,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -761,7 +774,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -779,7 +792,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -795,7 +808,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -811,7 +824,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>47</v>
       </c>
@@ -827,7 +840,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>48</v>
       </c>
@@ -843,7 +856,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>49</v>
       </c>
@@ -859,7 +872,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -875,7 +888,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -891,7 +904,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>52</v>
       </c>
@@ -907,7 +920,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -923,7 +936,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -939,7 +952,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>55</v>
       </c>
@@ -955,7 +968,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>56</v>
       </c>
@@ -971,7 +984,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>57</v>
       </c>
@@ -987,7 +1000,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="16.8">
       <c r="A24" t="s">
         <v>58</v>
       </c>

</xml_diff>